<commit_message>
make png and phina.js
</commit_message>
<xml_diff>
--- a/otherPage/rabbitShooting/doc/設計_画像.xlsx
+++ b/otherPage/rabbitShooting/doc/設計_画像.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\vbbeatProject\homePage\otherPage\rabbitShooting\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3E54E3-A10E-4429-B257-D251883A6F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48DE3A4-7812-4B91-B789-C705C2CDEF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="画像一覧" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="96">
   <si>
     <t>img</t>
     <phoneticPr fontId="1"/>
@@ -500,6 +500,13 @@
     <rPh sb="0" eb="3">
       <t>サクセイズ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>△</t>
+  </si>
+  <si>
+    <t>△</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -507,7 +514,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -521,6 +528,13 @@
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="2">
@@ -543,8 +557,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -829,674 +844,678 @@
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="4" max="4" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="8.796875" style="1"/>
+    <col min="4" max="4" width="12.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="8.796875" style="1"/>
+    <col min="11" max="11" width="8.69921875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3">
+      <c r="B3" s="1">
         <f>COUNTIF(B6:B61,"○")</f>
-        <v>41</v>
-      </c>
-      <c r="C3">
+        <v>31</v>
+      </c>
+      <c r="C3" s="1">
         <f>COUNTIF(C6:C61, "○")</f>
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:11">
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="9" spans="2:11">
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="B9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:11">
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="11" spans="2:11">
-      <c r="B11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="B11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="12" spans="2:11">
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:11">
-      <c r="B13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="B13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="2:11">
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="B14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="15" spans="2:11">
-      <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="B15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="2:11">
-      <c r="B16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="B16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="17" spans="2:11">
-      <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="B17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="18" spans="2:11">
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="B18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="19" spans="2:11">
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="20" spans="2:11">
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="21" spans="2:11">
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="22" spans="2:11">
-      <c r="B22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="B22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K22" t="s">
+      <c r="K22" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="23" spans="2:11">
-      <c r="B23" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="B23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="24" spans="2:11">
-      <c r="B24" t="s">
-        <v>38</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="B24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="25" spans="2:11">
-      <c r="B25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="B25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="26" spans="2:11">
-      <c r="B26" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="B26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K26" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="27" spans="2:11">
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28" spans="2:11">
-      <c r="B28" t="s">
-        <v>38</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="B28" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K28" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="29" spans="2:11">
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J29" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="30" spans="2:11">
-      <c r="B30" t="s">
-        <v>38</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="B30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K30" t="s">
+      <c r="K30" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="31" spans="2:11">
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="32" spans="2:11">
-      <c r="B32" t="s">
-        <v>38</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="B32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K32" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="33" spans="2:11">
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J33" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="34" spans="2:11">
-      <c r="B34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="B34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K34" t="s">
+      <c r="K34" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="35" spans="2:11">
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J35" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="36" spans="2:11">
-      <c r="B36" t="s">
-        <v>38</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="B36" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K36" t="s">
+      <c r="K36" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="37" spans="2:11">
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J37" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="38" spans="2:11">
-      <c r="B38" t="s">
-        <v>38</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="B38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K38" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="39" spans="2:11">
-      <c r="B39" t="s">
-        <v>38</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="B39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K39" t="s">
+      <c r="K39" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="40" spans="2:11">
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J40" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="41" spans="2:11">
-      <c r="B41" t="s">
-        <v>38</v>
-      </c>
-      <c r="F41" t="s">
+      <c r="B41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K41" t="s">
+      <c r="K41" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="42" spans="2:11">
-      <c r="B42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="B42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K42" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="43" spans="2:11">
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I43" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="44" spans="2:11">
-      <c r="B44" t="s">
-        <v>38</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="B44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J44" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="45" spans="2:11">
-      <c r="B45" t="s">
-        <v>38</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="B45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J45" t="s">
+      <c r="J45" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="46" spans="2:11">
-      <c r="B46" t="s">
-        <v>38</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="B46" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J46" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="47" spans="2:11">
-      <c r="B47" t="s">
-        <v>38</v>
-      </c>
-      <c r="E47" t="s">
+      <c r="B47" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J47" t="s">
+      <c r="J47" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="48" spans="2:11">
-      <c r="B48" t="s">
-        <v>38</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="B48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J48" t="s">
+      <c r="J48" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="49" spans="2:10">
-      <c r="B49" t="s">
-        <v>38</v>
-      </c>
-      <c r="E49" t="s">
+      <c r="B49" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J49" t="s">
+      <c r="J49" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="50" spans="2:10">
-      <c r="B50" t="s">
-        <v>38</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="B50" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J50" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="51" spans="2:10">
-      <c r="B51" t="s">
+      <c r="B51" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I51" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="2:10">
-      <c r="B52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="B52" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J52" t="s">
+      <c r="J52" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="53" spans="2:10">
-      <c r="B53" t="s">
-        <v>38</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="B53" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J53" t="s">
+      <c r="J53" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="54" spans="2:10">
-      <c r="B54" t="s">
-        <v>38</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="B54" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J54" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="55" spans="2:10">
-      <c r="B55" t="s">
+      <c r="B55" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I55" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="56" spans="2:10">
-      <c r="B56" t="s">
-        <v>38</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="B56" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J56" t="s">
+      <c r="J56" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="57" spans="2:10">
-      <c r="B57" t="s">
-        <v>38</v>
-      </c>
-      <c r="E57" t="s">
+      <c r="B57" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J57" t="s">
+      <c r="J57" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="58" spans="2:10">
-      <c r="B58" t="s">
-        <v>38</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="B58" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J58" t="s">
+      <c r="J58" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="59" spans="2:10">
-      <c r="B59" t="s">
-        <v>38</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="B59" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J59" t="s">
+      <c r="J59" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="60" spans="2:10">
-      <c r="B60" t="s">
+      <c r="B60" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I60" t="s">
+      <c r="I60" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="61" spans="2:10">
-      <c r="B61" t="s">
-        <v>38</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="B61" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J61" t="s">
+      <c r="J61" s="1" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="73" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>